<commit_message>
add new tests & TODOs
</commit_message>
<xml_diff>
--- a/tests/test_xlsx_2.xlsx
+++ b/tests/test_xlsx_2.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22513"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A4D1770D-36BB-4AF3-95B0-BCEBABC4321A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBF136D2-7E0A-4C5B-87CF-EF8030CE2A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -145,6 +147,15 @@
   </si>
   <si>
     <t>Colander</t>
+  </si>
+  <si>
+    <t>Blah</t>
+  </si>
+  <si>
+    <t>Ough</t>
+  </si>
+  <si>
+    <t>IM a new row</t>
   </si>
 </sst>
 </file>
@@ -498,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -817,4 +828,650 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DA58DB-86F7-4F44-9E7B-41409A05CFD1}">
+  <dimension ref="B2:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D697263D-E984-4501-9F0D-CBA09FDE85BE}">
+  <dimension ref="B2:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add code to check for new/deleted/renamed sheets (needs testing)
</commit_message>
<xml_diff>
--- a/tests/test_xlsx_2.xlsx
+++ b/tests/test_xlsx_2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22515"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD1990F5-F66A-4B43-A6F6-6B4E202137DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA005319-DB26-435A-B926-19210C91CBA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetA" sheetId="1" r:id="rId1"/>
-    <sheet name="SRAB" sheetId="2" r:id="rId2"/>
+    <sheet name="RNAME" sheetId="2" r:id="rId2"/>
     <sheet name="CCC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
@@ -834,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DA58DB-86F7-4F44-9E7B-41409A05CFD1}">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1156,7 +1156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D697263D-E984-4501-9F0D-CBA09FDE85BE}">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add deleted, new, renamed sheets to output
</commit_message>
<xml_diff>
--- a/tests/test_xlsx_2.xlsx
+++ b/tests/test_xlsx_2.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22515"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA005319-DB26-435A-B926-19210C91CBA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BAECAC3-1F71-4027-818B-B3C414255440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetA" sheetId="1" r:id="rId1"/>
     <sheet name="RNAME" sheetId="2" r:id="rId2"/>
     <sheet name="CCC" sheetId="3" r:id="rId3"/>
+    <sheet name="NSheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -834,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DA58DB-86F7-4F44-9E7B-41409A05CFD1}">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1474,4 +1475,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814E801A-7D0F-442F-8C88-BD977DD6D8B5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>